<commit_message>
fix: added row_id and converted child_id back to text
</commit_message>
<xml_diff>
--- a/dictionaries/outcome/1_2/1_2_mc_nonrep.xlsx
+++ b/dictionaries/outcome/1_2/1_2_mc_nonrep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\kaappi.oulu.fi\nfbc$\projects\P0511\Justiina\methylclock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/Visual/ds-dictionaries/dictionaries/outcome/1_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF2E5E3-40D7-4B88-B23E-68A6836418F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F56270-B99C-AC44-981C-F3322A7298F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33640" yWindow="-3820" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>Chronological gestational age (in weeks) at the time of DNA methylation measurement in methylclock</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>row_id</t>
+  </si>
+  <si>
+    <t>Unique identifier for the row in Opal</t>
   </si>
 </sst>
 </file>
@@ -231,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -239,11 +248,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -253,6 +277,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1425,21 +1451,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP22"/>
+  <dimension ref="A1:IP23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="4" customWidth="1"/>
-    <col min="5" max="250" width="8.85546875" style="4" customWidth="1"/>
-    <col min="251" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="4" customWidth="1"/>
+    <col min="5" max="250" width="8.83203125" style="4" customWidth="1"/>
+    <col min="251" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1453,51 +1481,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -1505,13 +1533,13 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1520,26 +1548,26 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
@@ -1548,12 +1576,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -1561,13 +1589,13 @@
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -1576,12 +1604,12 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -1589,13 +1617,13 @@
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1604,12 +1632,12 @@
         <v>4</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
@@ -1617,13 +1645,13 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
@@ -1632,12 +1660,12 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>7</v>
@@ -1645,13 +1673,13 @@
       <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
@@ -1660,12 +1688,12 @@
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -1674,12 +1702,12 @@
         <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>7</v>
@@ -1687,13 +1715,13 @@
       <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
@@ -1702,12 +1730,12 @@
         <v>4</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>7</v>
@@ -1716,34 +1744,48 @@
         <v>4</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1762,12 +1804,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
@@ -1782,7 +1824,7 @@
       </c>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1797,7 +1839,7 @@
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1812,7 +1854,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1827,7 +1869,7 @@
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1842,7 +1884,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1857,7 +1899,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1872,7 +1914,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1887,7 +1929,7 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1902,7 +1944,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1917,7 +1959,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>